<commit_message>
fix(ML): Linear, Ridge, Lasso, Logistic regression
</commit_message>
<xml_diff>
--- a/Concepts/Regression/LM-Training Process.xlsx
+++ b/Concepts/Regression/LM-Training Process.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\RahulAggarwal_Important\GITHUB\DataSciencePython\Concepts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\Rahul\DataSciencePython\Concepts\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -644,7 +644,7 @@
         <v>66666</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J3:J6" si="0">B5-I5</f>
+        <f t="shared" ref="J5:J6" si="0">B5-I5</f>
         <v>-5479</v>
       </c>
     </row>
@@ -861,7 +861,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>